<commit_message>
config file based on param 312
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roshan Manellore\Google Drive\Others\Python\GoldrattSim\GoldrattSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA9D6CD-53F8-47A0-820A-CCD2A88B9064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C83DFE0-8893-4E9F-8F6B-AC2BDBD914A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="helper" sheetId="4" r:id="rId1"/>
     <sheet name="Machines" sheetId="1" r:id="rId2"/>
-    <sheet name="Layout" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Financial" sheetId="7" r:id="rId3"/>
+    <sheet name="Layout" sheetId="2" r:id="rId4"/>
+    <sheet name="tasks" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1 (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Machine</t>
   </si>
@@ -89,36 +91,18 @@
     <t>RM</t>
   </si>
   <si>
-    <t>1,10,4</t>
-  </si>
-  <si>
     <t>Demand Format - id,quantity, selling price</t>
   </si>
   <si>
     <t>RM Format - id, quanity, cost price</t>
   </si>
   <si>
-    <t>3,10,4</t>
-  </si>
-  <si>
-    <t>4,10,4</t>
-  </si>
-  <si>
-    <t>5,20,100</t>
-  </si>
-  <si>
-    <t>7,20,100</t>
-  </si>
-  <si>
     <t>ID available</t>
   </si>
   <si>
     <t>ID used</t>
   </si>
   <si>
-    <t>9,20,100</t>
-  </si>
-  <si>
     <t>Yellow- ID used once</t>
   </si>
   <si>
@@ -131,36 +115,15 @@
     <t>H</t>
   </si>
   <si>
-    <t>Workstation Format-ID,machine color, run time, inventory_buffer, predecessor, successor</t>
-  </si>
-  <si>
-    <t>11,34,21</t>
-  </si>
-  <si>
-    <t>10,RED,20,0,1,5</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
     <t>multiple predecessors and successors can be given by separating by -</t>
   </si>
   <si>
-    <t>42,RED,20,0,4-3,11</t>
-  </si>
-  <si>
-    <t>8,BLUE,10,5,3,9-11-7</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
-    <t>add buffer box</t>
-  </si>
-  <si>
-    <t>display text in demand,warehouse and workstations</t>
-  </si>
-  <si>
     <t>button to toggle display in demand and RM</t>
   </si>
   <si>
@@ -173,12 +136,6 @@
     <t>Simulation pane</t>
   </si>
   <si>
-    <t>simulation toggle button</t>
-  </si>
-  <si>
-    <t>Workstation</t>
-  </si>
-  <si>
     <t>Time spent so far</t>
   </si>
   <si>
@@ -186,13 +143,133 @@
   </si>
   <si>
     <t>hrs</t>
+  </si>
+  <si>
+    <t>Popup</t>
+  </si>
+  <si>
+    <t>set values of RM</t>
+  </si>
+  <si>
+    <t>Limit for workstation</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>(25,26),(52,52))</t>
+  </si>
+  <si>
+    <t>Workstation Format-ID,machine color, run time, inventory_buffer, upsteam ID , downstream ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>statistics</t>
+  </si>
+  <si>
+    <t>for end of day - optional</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Opening Balance</t>
+  </si>
+  <si>
+    <t>Fixed Cash</t>
+  </si>
+  <si>
+    <t>1,0,30</t>
+  </si>
+  <si>
+    <t>2,0,35</t>
+  </si>
+  <si>
+    <t>3,0,30</t>
+  </si>
+  <si>
+    <t>4,0,65</t>
+  </si>
+  <si>
+    <t>12,CYAN,9,0,3,20</t>
+  </si>
+  <si>
+    <t>11,GREEN,5,0,2,30</t>
+  </si>
+  <si>
+    <t>10,GREEN,4,0,1,30</t>
+  </si>
+  <si>
+    <t>20,PINK,18,15,12,52</t>
+  </si>
+  <si>
+    <t>13,GREEN,15,0,4,21</t>
+  </si>
+  <si>
+    <t>100,40,180</t>
+  </si>
+  <si>
+    <t>101,50,240</t>
+  </si>
+  <si>
+    <t>102,40,180</t>
+  </si>
+  <si>
+    <t>30,BROWN,8,25,10-11,50-51</t>
+  </si>
+  <si>
+    <t>31,PINK,20,10,21,53</t>
+  </si>
+  <si>
+    <t>53,BLUE,14,0,31,72</t>
+  </si>
+  <si>
+    <t>50,GREEN,15,0,30,60</t>
+  </si>
+  <si>
+    <t>51,BLUE,6,0,30,71</t>
+  </si>
+  <si>
+    <t>52,BLUE,28,0,20,71</t>
+  </si>
+  <si>
+    <t>60,CYAN,15,0,50,70</t>
+  </si>
+  <si>
+    <t>70,PINK,20,0,60,90</t>
+  </si>
+  <si>
+    <t>71,BROWN,9,0,51-52,91</t>
+  </si>
+  <si>
+    <t>72,PINK,7,0,53,92</t>
+  </si>
+  <si>
+    <t>90,CYAN,18,0,70,100</t>
+  </si>
+  <si>
+    <t>92,CYAN,10,0,72,102</t>
+  </si>
+  <si>
+    <t>21,CYAN,12,0,13,31</t>
+  </si>
+  <si>
+    <t>91,CYAN,6,0,71,101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +290,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -241,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -342,11 +425,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -369,34 +461,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -422,6 +502,414 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C842B56-E37C-4203-BB98-4D54F616BC79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9174480" y="998220"/>
+          <a:ext cx="7193280" cy="4419600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{950B91C1-265A-40AC-899F-D98432C7031C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10812780" y="220980"/>
+          <a:ext cx="7216140" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380D044A-8C3B-4DDA-A77A-21310B0AB224}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="6642" t="11749" r="4175" b="6292"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9136380" y="1028700"/>
+          <a:ext cx="7216140" cy="4391098"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B0A2795-8D1E-451B-8245-246C9F6B3331}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9151620" y="1066800"/>
+          <a:ext cx="7216140" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB2B234C-DE0E-4A06-8A57-72D195DCA324}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7391400" y="1874520"/>
+          <a:ext cx="7216140" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C445066-A460-449E-AB79-82F506020DED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7764780" y="60960"/>
+          <a:ext cx="7193280" cy="4419600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Oval 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF1DAA0-99F2-4A66-8D7B-B81EDAACB277}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9204960" y="1097280"/>
+          <a:ext cx="7124700" cy="4244340"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF100B84-E14A-4BB3-ABDF-2FA9099A0861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9700260" y="2308860"/>
+          <a:ext cx="7193280" cy="4419600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -717,7 +1205,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -735,13 +1223,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -757,35 +1248,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>20</v>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -806,11 +1319,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520D1FD3-DAEF-4F0F-A19E-BBCB4D5EE6EA}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>11000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF48F47-F38B-407F-8804-435F5EF02A3D}">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,51 +1400,49 @@
         <v>14</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="V1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
+      <c r="K1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="V1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="16"/>
+      <c r="B2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="2"/>
       <c r="K2">
         <v>1</v>
@@ -934,31 +1485,31 @@
       <c r="U2" s="3"/>
       <c r="V2" t="str">
         <f t="shared" ref="V2:AC2" si="1">IFERROR(LEFT(B2,FIND(",",B2)-1),"")</f>
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="W2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="X2" t="str">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>IFERROR(LEFT(D2,FIND(",",D2)-1),"")</f>
+        <v/>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f>IFERROR(LEFT(E2,FIND(",",E2)-1),"")</f>
+        <v>101</v>
       </c>
       <c r="Z2" t="str">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v/>
       </c>
       <c r="AA2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>102</v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC2" t="str">
         <f t="shared" si="1"/>
@@ -973,14 +1524,20 @@
       <c r="A3" s="6">
         <v>9</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="B3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
       <c r="J3" s="2"/>
       <c r="K3">
         <v>2</v>
@@ -1023,7 +1580,7 @@
       <c r="U3" s="3"/>
       <c r="V3" t="str">
         <f t="shared" ref="V3:V12" si="6">IFERROR(LEFT(B3,FIND(",",B3)-1),"")</f>
-        <v/>
+        <v>90</v>
       </c>
       <c r="W3" t="str">
         <f t="shared" ref="W3:W12" si="7">IFERROR(LEFT(C3,FIND(",",C3)-1),"")</f>
@@ -1035,7 +1592,7 @@
       </c>
       <c r="Y3" t="str">
         <f t="shared" ref="Y3:Y12" si="9">IFERROR(LEFT(E3,FIND(",",E3)-1),"")</f>
-        <v/>
+        <v>91</v>
       </c>
       <c r="Z3" t="str">
         <f t="shared" ref="Z3:Z12" si="10">IFERROR(LEFT(F3,FIND(",",F3)-1),"")</f>
@@ -1043,7 +1600,7 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" ref="AA3:AA12" si="11">IFERROR(LEFT(G3,FIND(",",G3)-1),"")</f>
-        <v/>
+        <v>92</v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" ref="AB3:AC12" si="12">IFERROR(LEFT(H3,FIND(",",H3)-1),"")</f>
@@ -1058,14 +1615,14 @@
       <c r="A4" s="6">
         <v>8</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="2"/>
       <c r="K4">
         <v>3</v>
@@ -1143,16 +1700,20 @@
       <c r="A5" s="6">
         <v>7</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2"/>
       <c r="K5">
         <v>4</v>
@@ -1195,7 +1756,7 @@
       <c r="U5" s="3"/>
       <c r="V5" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>70</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="7"/>
@@ -1207,7 +1768,7 @@
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="9"/>
-        <v/>
+        <v>71</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="10"/>
@@ -1215,7 +1776,7 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="12"/>
@@ -1230,14 +1791,16 @@
       <c r="A6" s="6">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="2"/>
       <c r="K6">
         <v>5</v>
@@ -1280,7 +1843,7 @@
       <c r="U6" s="3"/>
       <c r="V6" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>60</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="7"/>
@@ -1315,14 +1878,22 @@
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="2"/>
       <c r="K7">
         <v>6</v>
@@ -1365,7 +1936,7 @@
       <c r="U7" s="3"/>
       <c r="V7" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>50</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="7"/>
@@ -1373,7 +1944,7 @@
       </c>
       <c r="X7" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>51</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="9"/>
@@ -1381,11 +1952,11 @@
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>52</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>53</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="12"/>
@@ -1400,18 +1971,14 @@
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="2"/>
       <c r="K8">
         <v>7</v>
@@ -1454,7 +2021,7 @@
       <c r="U8" s="3"/>
       <c r="V8" t="str">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="7"/>
@@ -1462,7 +2029,7 @@
       </c>
       <c r="X8" t="str">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="9"/>
@@ -1489,14 +2056,18 @@
       <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="2"/>
       <c r="K9">
         <v>8</v>
@@ -1543,7 +2114,7 @@
       </c>
       <c r="W9" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>30</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="8"/>
@@ -1559,7 +2130,7 @@
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>31</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="12"/>
@@ -1574,14 +2145,18 @@
       <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="2"/>
       <c r="K10">
         <v>9</v>
@@ -1640,11 +2215,11 @@
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>20</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>21</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="12"/>
@@ -1659,14 +2234,22 @@
       <c r="A11" s="6">
         <v>1</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="B11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="2"/>
       <c r="K11">
         <v>10</v>
@@ -1709,7 +2292,7 @@
       <c r="U11" s="3"/>
       <c r="V11" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="7"/>
@@ -1717,7 +2300,7 @@
       </c>
       <c r="X11" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="9"/>
@@ -1725,11 +2308,11 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>12</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="12"/>
@@ -1744,20 +2327,22 @@
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="18"/>
+      <c r="B12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="2"/>
       <c r="K12">
         <v>11</v>
@@ -1808,7 +2393,7 @@
       </c>
       <c r="X12" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="9"/>
@@ -1816,15 +2401,15 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="AC12" t="str">
         <f t="shared" si="12"/>
@@ -1833,17 +2418,17 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1854,26 +2439,29 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+    <row r="17" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>35</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J24" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1894,56 +2482,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E4DE47-2BFF-4ED2-824D-E0987B5CBB03}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="I2">
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>39</v>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>40</v>
+      <c r="H4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>44</v>
+      <c r="C8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1951,17 +2547,776 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>41</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA67800-6791-42E1-90FE-EB6F17E61892}">
+  <dimension ref="A1:BY36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="16" max="65" width="2.109375" customWidth="1"/>
+    <col min="71" max="72" width="4.88671875" customWidth="1"/>
+    <col min="77" max="77" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>6</v>
+      </c>
+      <c r="V3">
+        <v>7</v>
+      </c>
+      <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
+        <v>9</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="Z3">
+        <v>11</v>
+      </c>
+      <c r="AA3">
+        <v>12</v>
+      </c>
+      <c r="AB3">
+        <v>13</v>
+      </c>
+      <c r="AC3">
+        <v>14</v>
+      </c>
+      <c r="AD3">
+        <v>15</v>
+      </c>
+      <c r="AE3">
+        <v>16</v>
+      </c>
+      <c r="AF3">
+        <v>17</v>
+      </c>
+      <c r="AG3">
+        <v>18</v>
+      </c>
+      <c r="AH3">
+        <v>19</v>
+      </c>
+      <c r="AI3">
+        <v>20</v>
+      </c>
+      <c r="AJ3">
+        <v>21</v>
+      </c>
+      <c r="AK3">
+        <v>22</v>
+      </c>
+      <c r="AL3">
+        <v>23</v>
+      </c>
+      <c r="AM3">
+        <v>24</v>
+      </c>
+      <c r="AN3">
+        <v>25</v>
+      </c>
+      <c r="AO3">
+        <v>26</v>
+      </c>
+      <c r="AP3">
+        <v>27</v>
+      </c>
+      <c r="AQ3">
+        <v>28</v>
+      </c>
+      <c r="AR3">
+        <v>29</v>
+      </c>
+      <c r="AS3">
+        <v>30</v>
+      </c>
+      <c r="AT3">
+        <v>31</v>
+      </c>
+      <c r="AU3">
+        <v>32</v>
+      </c>
+      <c r="AV3">
+        <v>33</v>
+      </c>
+      <c r="AW3">
+        <v>34</v>
+      </c>
+      <c r="AX3">
+        <v>35</v>
+      </c>
+      <c r="AY3">
+        <v>36</v>
+      </c>
+      <c r="AZ3">
+        <v>37</v>
+      </c>
+      <c r="BA3">
+        <v>38</v>
+      </c>
+      <c r="BB3">
+        <v>39</v>
+      </c>
+      <c r="BC3">
+        <v>40</v>
+      </c>
+      <c r="BD3">
+        <v>41</v>
+      </c>
+      <c r="BE3">
+        <v>42</v>
+      </c>
+      <c r="BF3">
+        <v>43</v>
+      </c>
+      <c r="BG3">
+        <v>44</v>
+      </c>
+      <c r="BH3">
+        <v>45</v>
+      </c>
+      <c r="BI3">
+        <v>46</v>
+      </c>
+      <c r="BJ3">
+        <v>47</v>
+      </c>
+      <c r="BK3">
+        <v>48</v>
+      </c>
+      <c r="BL3">
+        <v>49</v>
+      </c>
+      <c r="BM3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <f>P4+1</f>
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:BM4" si="0">Q4+1</f>
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AB4">
+        <f>AA4+1</f>
+        <v>13</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AM4">
+        <f>AL4+1</f>
+        <v>24</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AS4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AT4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AU4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AV4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AW4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AX4">
+        <f>AW4+1</f>
+        <v>35</v>
+      </c>
+      <c r="AY4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AZ4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="BA4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="BB4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="BC4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="BD4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="BE4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="BF4">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="BG4">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="BH4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="BI4">
+        <f>BH4+1</f>
+        <v>46</v>
+      </c>
+      <c r="BJ4">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="BK4">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="BL4">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="BM4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="BY5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="BQ7">
+        <v>22</v>
+      </c>
+      <c r="BR7">
+        <v>1</v>
+      </c>
+      <c r="BS7">
+        <f>BR7+26</f>
+        <v>27</v>
+      </c>
+      <c r="BU7">
+        <v>49</v>
+      </c>
+      <c r="BV7">
+        <v>18</v>
+      </c>
+      <c r="BW7">
+        <f>BV7+26</f>
+        <v>44</v>
+      </c>
+      <c r="BY7" t="str">
+        <f>"pygame.draw.aaline(self.sur,BLACK,"&amp;"("&amp;BQ7&amp;","&amp;BS7&amp;"),("&amp;BU7&amp;","&amp;BW7&amp;"))"</f>
+        <v>pygame.draw.aaline(self.sur,BLACK,(22,27),(49,44))</v>
+      </c>
+    </row>
+    <row r="8" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <f>O7+1</f>
+        <v>2</v>
+      </c>
+      <c r="BQ8">
+        <v>8</v>
+      </c>
+      <c r="BR8">
+        <v>5</v>
+      </c>
+      <c r="BS8">
+        <f t="shared" ref="BS8:BS12" si="1">BR8+26</f>
+        <v>31</v>
+      </c>
+      <c r="BU8">
+        <v>42</v>
+      </c>
+      <c r="BV8">
+        <v>26</v>
+      </c>
+      <c r="BW8">
+        <f t="shared" ref="BW8:BW12" si="2">BV8+26</f>
+        <v>52</v>
+      </c>
+      <c r="BY8" t="str">
+        <f t="shared" ref="BY8:BY12" si="3">"pygame.draw.aaline(self.sur,BLACK,"&amp;"("&amp;BQ8&amp;","&amp;BS8&amp;"),("&amp;BU8&amp;","&amp;BW8&amp;"))"</f>
+        <v>pygame.draw.aaline(self.sur,BLACK,(8,31),(42,52))</v>
+      </c>
+    </row>
+    <row r="9" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <f t="shared" ref="O9:O36" si="4">O8+1</f>
+        <v>3</v>
+      </c>
+      <c r="BQ9">
+        <v>1</v>
+      </c>
+      <c r="BR9">
+        <v>14</v>
+      </c>
+      <c r="BS9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="BU9">
+        <v>29</v>
+      </c>
+      <c r="BV9">
+        <v>30</v>
+      </c>
+      <c r="BW9">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="BY9" t="str">
+        <f t="shared" si="3"/>
+        <v>pygame.draw.aaline(self.sur,BLACK,(1,40),(29,56))</v>
+      </c>
+    </row>
+    <row r="10" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="BQ10">
+        <v>29</v>
+      </c>
+      <c r="BR10">
+        <v>1</v>
+      </c>
+      <c r="BS10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="BU10">
+        <v>2</v>
+      </c>
+      <c r="BV10">
+        <v>18</v>
+      </c>
+      <c r="BW10">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="BY10" t="str">
+        <f t="shared" si="3"/>
+        <v>pygame.draw.aaline(self.sur,BLACK,(29,27),(2,44))</v>
+      </c>
+    </row>
+    <row r="11" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="BQ11">
+        <v>43</v>
+      </c>
+      <c r="BR11">
+        <v>5</v>
+      </c>
+      <c r="BS11">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="BU11">
+        <v>8</v>
+      </c>
+      <c r="BV11">
+        <v>26</v>
+      </c>
+      <c r="BW11">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="BY11" t="str">
+        <f t="shared" si="3"/>
+        <v>pygame.draw.aaline(self.sur,BLACK,(43,31),(8,52))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="BQ12">
+        <v>49</v>
+      </c>
+      <c r="BR12">
+        <v>14</v>
+      </c>
+      <c r="BS12">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="BU12">
+        <v>21</v>
+      </c>
+      <c r="BV12">
+        <v>29</v>
+      </c>
+      <c r="BW12">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="BY12" t="str">
+        <f t="shared" si="3"/>
+        <v>pygame.draw.aaline(self.sur,BLACK,(49,40),(21,55))</v>
+      </c>
+    </row>
+    <row r="13" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:77" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>104714</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>100*10</f>
+        <v>1000</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>A17+A16</f>
+        <v>105714</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O21">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O22">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O23">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O28">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O29">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O30">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O31">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O32">
+        <f>O31+1</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="15:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O33">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O34">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O35">
+        <f>O34+1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="15:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O36">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>